<commit_message>
Clean up muni_election folder
</commit_message>
<xml_diff>
--- a/data/municipal_elections/Sources_overview.xlsx
+++ b/data/municipal_elections/Sources_overview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flosic/Documents/GitHub/german_election_data/data/municipal_elections/archive/final_output/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flosic/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27E8E18A-FA99-6849-B820-B5852E0FD39F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E82F16-02E7-FD41-84DB-E8D7803D422E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4380" yWindow="-21100" windowWidth="38400" windowHeight="20200" xr2:uid="{226FADFE-BBFE-E444-B07F-A513505EA323}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{226FADFE-BBFE-E444-B07F-A513505EA323}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
   <si>
     <t>Source</t>
   </si>
@@ -48,21 +48,12 @@
     <t>Bayern</t>
   </si>
   <si>
-    <t>https://statistik.hessen.de/zahlen-fakten/kommunalwahlen</t>
-  </si>
-  <si>
-    <t>https://www.statistikdaten.bayern.de/genesis/online?operation=themes&amp;levelindex=0&amp;levelid=1638980673533&amp;code=14#abreadcrumb</t>
-  </si>
-  <si>
     <t>Hessen</t>
   </si>
   <si>
     <t>Thueringen</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.wahlen.thueringen.de/kommunalwahlen/kw_wahlergebnisse_GW.asp </t>
-  </si>
-  <si>
     <t>BW</t>
   </si>
   <si>
@@ -78,9 +69,6 @@
     <t>Hamburg</t>
   </si>
   <si>
-    <t>https://www.statistik-nord.de/wahlen/wahlen-in-hamburg/buergerschaftswahlen/2020#c8007</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
@@ -96,56 +84,80 @@
     <t>Niedersachsen</t>
   </si>
   <si>
-    <t>https://www.statistik.niedersachsen.de/startseite/themen/wahlen/wahlen-in-niedersachsen-statistische-berichte-b-vii-3-179044.html</t>
-  </si>
-  <si>
     <t>Baden-Wuerttemberg</t>
   </si>
   <si>
     <t>Schleswig-Holstein</t>
   </si>
   <si>
-    <t>https://www.statistischebibliothek.de/mir/receive/SHSerie_mods_00000466</t>
-  </si>
-  <si>
-    <t>https://www.statistik.sachsen.de/genonline/online?operation=find&amp;suchanweisung_language=de&amp;query=14431#abreadcrumb</t>
-  </si>
-  <si>
     <t>Bremen</t>
   </si>
   <si>
-    <t>https://www.statistik.bremen.de/datenangebote-8409</t>
-  </si>
-  <si>
-    <t>https://www.statistik-berlin-brandenburg.de/kommunalwahlen/</t>
-  </si>
-  <si>
     <t>Mecklenburg Vorpommern</t>
   </si>
   <si>
-    <t>before 2003 (1998 and 1993) only scanned PDFs</t>
-  </si>
-  <si>
-    <t>https://www.laiv-mv.de/Statistik/Zahlen-und-Fakten/Gesellschaft-&amp;-Staat/Wahlen-&amp;-Volksabstimmungen</t>
-  </si>
-  <si>
-    <t>email for before 2006</t>
-  </si>
-  <si>
-    <t>https://wahlergebnisse.sachsen-anhalt.de/wahlen/kw19/and/kw.download.html</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>available and processed for 2008 and 2018; machine-readable PDF for 2003; scanned PDFs before that; 2013 sent via Email from Statistikamt Nord</t>
+    <t>Bayerisches Landesamt für Statistik</t>
+  </si>
+  <si>
+    <t>Amt für Statistik Berlin-Brandenburg</t>
+  </si>
+  <si>
+    <t>Statistisches Landesamt Bremen</t>
+  </si>
+  <si>
+    <t>Statistisches Landesamt Baden-Württemberg</t>
+  </si>
+  <si>
+    <t>Procured via</t>
+  </si>
+  <si>
+    <t>website</t>
+  </si>
+  <si>
+    <t>Statistik Nord</t>
+  </si>
+  <si>
+    <t>Hessisches Statistisches Landesamt</t>
+  </si>
+  <si>
+    <t>Mecklenburg-Vorpommern Landesamt für innere Verwaltung Statistisches Amt</t>
+  </si>
+  <si>
+    <t>Landesamt für Statistik Niedersachsen</t>
+  </si>
+  <si>
+    <t>website after 2006; email before 2006</t>
+  </si>
+  <si>
+    <t>Statistisches Landesamt Nordrhein-Westfalen</t>
+  </si>
+  <si>
+    <t>Statistisches Landesamt Rheinland-Pfalz</t>
+  </si>
+  <si>
+    <t>Statistisches Landesamt des Saarlandes</t>
+  </si>
+  <si>
+    <t>Statistisches Landesamt des Freistaates Sachsen</t>
+  </si>
+  <si>
+    <t>Statistisches Landesamt Sachsen-Anhalt</t>
+  </si>
+  <si>
+    <t>Statistisches Amt für Hamburg und Schleswig-Holstein</t>
+  </si>
+  <si>
+    <t>Thüringer Landesamt für Statistik</t>
+  </si>
+  <si>
+    <t>website except for 2013; email for 2013</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -157,14 +169,6 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -187,17 +191,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -513,13 +514,14 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="116.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.5" customWidth="1"/>
+    <col min="3" max="3" width="34.6640625" customWidth="1"/>
     <col min="4" max="4" width="116.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -531,15 +533,18 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -547,136 +552,175 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="2" t="s">
         <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
         <v>27</v>
       </c>
-      <c r="B9" t="s">
-        <v>29</v>
+      <c r="C9" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
         <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>33</v>
+      </c>
+      <c r="C14" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>34</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B8" r:id="rId1" tooltip="https://statistik.hessen.de/zahlen-fakten/kommunalwahlen" xr:uid="{1D9A2FC2-8512-9942-8F8F-397AE5277A7F}"/>
-    <hyperlink ref="B16" r:id="rId2" xr:uid="{4A0ED774-FE99-8D40-B9A8-0DBDBA3E8538}"/>
-    <hyperlink ref="B17" r:id="rId3" xr:uid="{8DFB7A3C-FD70-EC48-AB8E-6D29204472F8}"/>
-    <hyperlink ref="B10" r:id="rId4" xr:uid="{E52DB018-FC44-4D4E-8A00-082386D2CF51}"/>
+    <hyperlink ref="B11" r:id="rId1" display="https://www.it.nrw/statistik" xr:uid="{B97BE82B-DD60-5C47-A580-FD63E01BAE08}"/>
+    <hyperlink ref="B12" r:id="rId2" display="https://www.statistik.rlp.de/" xr:uid="{2A8C499A-F1A2-524E-A66D-22D2C83D17CD}"/>
+    <hyperlink ref="B13" r:id="rId3" display="https://www.saarland.de/stat/DE/home" xr:uid="{4807CBDF-2D99-3B4B-8DCF-C0BB0A09EAB8}"/>
+    <hyperlink ref="B15" r:id="rId4" display="https://statistik.sachsen-anhalt.de/" xr:uid="{6516FE97-BFF8-334F-968E-840A3DD2CAC8}"/>
+    <hyperlink ref="B16" r:id="rId5" display="https://www.statistik-nord.de/" xr:uid="{691ACDD3-FFB9-4C4A-9738-AA23F65621A6}"/>
+    <hyperlink ref="B17" r:id="rId6" display="https://statistik.thueringen.de/" xr:uid="{09F198DA-E8D8-924F-A35A-9C085FBE9BAE}"/>
+    <hyperlink ref="B2" r:id="rId7" display="https://www.statistik-bw.de/" xr:uid="{4F3BEF15-421E-784C-AFAE-6B27DD001497}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>